<commit_message>
better dataclass solution for activities
</commit_message>
<xml_diff>
--- a/model_parameters/Road_dust_parameter_table_v11.xlsx
+++ b/model_parameters/Road_dust_parameter_table_v11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindredenby/Documents/metrologisk/NORTRIP-python/model_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0D0ADC-8E05-3B4E-8225-792A1358B297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D2EDFA-E0E2-064C-A65C-DF1F9CE9CE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="-960" windowWidth="33600" windowHeight="19240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10554,8 +10554,8 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
summary changes and polish
</commit_message>
<xml_diff>
--- a/model_parameters/Road_dust_parameter_table_v11.xlsx
+++ b/model_parameters/Road_dust_parameter_table_v11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindredenby/Documents/metrologisk/NORTRIP-python/model_parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F587D0-30CD-2542-B9FD-579B7EF6D490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B3EADF-B590-3A44-9FA5-E5B2E7CBA85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="-19840" windowWidth="30340" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21000" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -5976,8 +5976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q190"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+    <sheetView topLeftCell="A143" zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9927,7 +9927,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>